<commit_message>
chore: updates to ARPA output templates for 2025 April
</commit_message>
<xml_diff>
--- a/packages/server/src/arpa_reporter/data/treasury/project111210BulkUpload.xlsx
+++ b/packages/server/src/arpa_reporter/data/treasury/project111210BulkUpload.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kgu82\Downloads\SLFRFBulkUploadTemplates\SLFRFBulkUploadTemplates\SLFRFBulkUploadTemplates\Quarter 4 2024 Project Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kgu82\Desktop\SLFRFBulkUploadTemplates\SLFRFBulkUploadTemplates\SLFRFBulkUploadTemplates\Quarter 1 2025 Project Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1D0E71B-572D-4458-908C-6EE36A4E507D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{878D997D-E936-4A76-B2F8-CED902FA064E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -475,10 +475,10 @@
 End date  Valid Date - (MM/DD/YYYY)</t>
   </si>
   <si>
-    <t>Q4_2024_Obligations__c</t>
+    <t>Q1_2025_Obligations__c</t>
   </si>
   <si>
-    <t>Q4_2024_Expenditures__c</t>
+    <t>Q1_2025_Expenditures__c</t>
   </si>
 </sst>
 </file>
@@ -37223,6 +37223,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FD7D29C8E3DCB740B512085BDB890A19" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="252040482c07e84078604bad08e1f478">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1998147e-1bae-4425-a5b5-824e2b69f76d" xmlns:ns3="79f0e6e4-ac4e-4584-83f0-2cc69c4e4aae" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a426bac492543af192e091bebadc75c6" ns2:_="" ns3:_="">
     <xsd:import namespace="1998147e-1bae-4425-a5b5-824e2b69f76d"/>
@@ -37439,22 +37454,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44B7B1D8-F3F2-46A8-A792-B679C78EEEEB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="79f0e6e4-ac4e-4584-83f0-2cc69c4e4aae"/>
+    <ds:schemaRef ds:uri="1998147e-1bae-4425-a5b5-824e2b69f76d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D55B629F-9BAD-43E6-819F-B097A47F8C05}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D20EFE-128A-4BEA-B77D-8F21601543E1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -37471,29 +37496,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D55B629F-9BAD-43E6-819F-B097A47F8C05}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44B7B1D8-F3F2-46A8-A792-B679C78EEEEB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="79f0e6e4-ac4e-4584-83f0-2cc69c4e4aae"/>
-    <ds:schemaRef ds:uri="1998147e-1bae-4425-a5b5-824e2b69f76d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
chore: add updated treasury report files
</commit_message>
<xml_diff>
--- a/packages/server/src/arpa_reporter/data/treasury/project111210BulkUpload.xlsx
+++ b/packages/server/src/arpa_reporter/data/treasury/project111210BulkUpload.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kgu82\Desktop\SLFRFBulkUploadTemplates\SLFRFBulkUploadTemplates\SLFRFBulkUploadTemplates\Quarter 1 2025 Project Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kgu82\Desktop\SLFRFBulkUploadTemplates\SLFRFBulkUploadTemplates\SLFRFBulkUploadTemplates\Quarter 2 2025 Project Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AC93BFE-EED7-4C7D-B79F-7A0464D61070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F32D2FC-A2C4-4337-BA6E-01A6175D8B5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17472" windowHeight="13704" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 " sheetId="2" r:id="rId1"/>
@@ -475,12 +475,6 @@
 End date  Valid Date - (MM/DD/YYYY)</t>
   </si>
   <si>
-    <t>Q1_2025_Obligations__c</t>
-  </si>
-  <si>
-    <t>Q1_2025_Expenditures__c</t>
-  </si>
-  <si>
     <t>Prog_Income_Earned_After_12_31_24__c</t>
   </si>
   <si>
@@ -497,6 +491,12 @@
   </si>
   <si>
     <t>Program Income reported after Q4 2024 expended</t>
+  </si>
+  <si>
+    <t>Q2_2025_Obligations__c</t>
+  </si>
+  <si>
+    <t>Q2_2025_Expenditures__c</t>
   </si>
 </sst>
 </file>
@@ -1111,10 +1111,10 @@
         <v>8</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="O4" s="3" t="s">
         <v>30</v>
@@ -1174,13 +1174,13 @@
         <v>76</v>
       </c>
       <c r="AH4" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="AI4" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="AJ4" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:36" ht="13.2" x14ac:dyDescent="0.25">
@@ -1394,13 +1394,13 @@
         <v>73</v>
       </c>
       <c r="AH6" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AI6" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="AJ6" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:36" ht="409.6" x14ac:dyDescent="0.25">
@@ -1504,13 +1504,13 @@
         <v>83</v>
       </c>
       <c r="AH7" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AI7" s="11" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="AJ7" s="11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:36" ht="43.35" customHeight="1" x14ac:dyDescent="0.25">
@@ -39255,6 +39255,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FD7D29C8E3DCB740B512085BDB890A19" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="252040482c07e84078604bad08e1f478">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1998147e-1bae-4425-a5b5-824e2b69f76d" xmlns:ns3="79f0e6e4-ac4e-4584-83f0-2cc69c4e4aae" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a426bac492543af192e091bebadc75c6" ns2:_="" ns3:_="">
     <xsd:import namespace="1998147e-1bae-4425-a5b5-824e2b69f76d"/>
@@ -39471,22 +39486,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44B7B1D8-F3F2-46A8-A792-B679C78EEEEB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="79f0e6e4-ac4e-4584-83f0-2cc69c4e4aae"/>
+    <ds:schemaRef ds:uri="1998147e-1bae-4425-a5b5-824e2b69f76d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D55B629F-9BAD-43E6-819F-B097A47F8C05}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D20EFE-128A-4BEA-B77D-8F21601543E1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -39503,29 +39528,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D55B629F-9BAD-43E6-819F-B097A47F8C05}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44B7B1D8-F3F2-46A8-A792-B679C78EEEEB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="79f0e6e4-ac4e-4584-83f0-2cc69c4e4aae"/>
-    <ds:schemaRef ds:uri="1998147e-1bae-4425-a5b5-824e2b69f76d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>